<commit_message>
Star City part 2
</commit_message>
<xml_diff>
--- a/Weather.xlsx
+++ b/Weather.xlsx
@@ -353,7 +353,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -386,7 +388,7 @@
         <v>42753</v>
       </c>
       <c r="B4">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>